<commit_message>
borrando runners para ahcer pruebas de jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Servicios.xlsx
+++ b/src/test/resources/excel/Servicios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Documents\banbif\CODIGO\serenity-cucumber-starter\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1530B7FB-2F12-402F-9B95-EE4D420D06AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC821D57-25ED-42B3-81D4-FE9CA325E3B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{0C197A92-FFFA-4A8E-9608-522EBB81720B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{0C197A92-FFFA-4A8E-9608-522EBB81720B}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" state="hidden" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4071" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4093" uniqueCount="766">
   <si>
     <t>TC</t>
   </si>
@@ -6344,12 +6344,54 @@
   <si>
     <t>/api-recaudaciones/v1/convenios/13</t>
   </si>
+  <si>
+    <t>Extornar Cuota Préstamo</t>
+  </si>
+  <si>
+    <t>https://apicast-pagos-3scale.uatapps.dombif.peru</t>
+  </si>
+  <si>
+    <t>/api-pagos/v1/extornos</t>
+  </si>
+  <si>
+    <t>{​​​​​"numeroSucursal":"4567","numeroCajero":"123","tipoTransaccionTeller":0,"cuentaPagare":{​​​​​"numero":"241130294760"}​​​​​,"fechaHoraProceso":"2019-04-15T19:05:01.548Z"}​​​​​</t>
+  </si>
+  <si>
+    <t>Content-Type:application/json;codigoCanal:BANCA_POR_INTERNET</t>
+  </si>
+  <si>
+    <t>Pagar Cuota Préstamo</t>
+  </si>
+  <si>
+    <t>https://apicast-pagos-3scale.uatapps.dombif.peru:443</t>
+  </si>
+  <si>
+    <t>/api-pagos/v1/pagos</t>
+  </si>
+  <si>
+    <t>{​​​​​"numeroSucursal":"1234","numeroCajero":"123","tipoTransaccionTeller":681,"cuentaPagare":{​​​​​"numero":"241130294760"}​​​​​,"cuotas":[{​​​​​"numero":1}​​​​​,{​​​​​"numero":2}​​​​​],"tipo":"REDUCE_CUOTA","tipoAfectacion":"CAPITAL_Y_INTERES","medioPago":"EFECTIVO","numeroLiquidacion":"","tipoCambio":0,"tarjeta":{​​​​​"numero":"0"}​​​​​,"cuentaCargo":{​​​​​"numero":"0"}​​​​​,"cheque":{​​​​​"numero":0}​​​​​,"monto":10000,"monedaMonto":"USD","concepto":{​​​​​"codigo":""}​​​​​}​​​​​</t>
+  </si>
+  <si>
+    <t>BPI-API PAGOS</t>
+  </si>
+  <si>
+    <t>PAGOS</t>
+  </si>
+  <si>
+    <t>https://ssorh.uatapps.dombif.peru</t>
+  </si>
+  <si>
+    <t>/auth/realms/Banbif-API/protocol/openid-connect/token</t>
+  </si>
+  <si>
+    <t>grant_type:client_credentials;client_id:b50d4eb0;client_secret:49a6edf565b35e211613130c34ff8390</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6438,6 +6480,24 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFDA846B"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF99B3D4"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -6541,7 +6601,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6680,6 +6740,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -11949,8 +12021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54966F88-D9D0-4CA2-9164-3EB81D4EEF31}">
   <dimension ref="A1:M113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD8"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12238,28 +12310,81 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25" t="s">
-        <v>252</v>
-      </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
+    <row r="9" spans="1:13" ht="33">
+      <c r="A9" s="86">
+        <v>11</v>
+      </c>
+      <c r="B9" s="86" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" s="86" t="s">
+        <v>752</v>
+      </c>
+      <c r="D9" s="86" t="s">
+        <v>269</v>
+      </c>
+      <c r="E9" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="87" t="s">
+        <v>753</v>
+      </c>
+      <c r="G9" s="86" t="s">
+        <v>754</v>
+      </c>
+      <c r="H9" s="85"/>
+      <c r="I9" s="86" t="s">
+        <v>755</v>
+      </c>
+      <c r="J9" s="86" t="s">
+        <v>756</v>
+      </c>
+      <c r="K9" s="86" t="s">
+        <v>500</v>
+      </c>
+      <c r="L9" s="86">
+        <v>400</v>
+      </c>
+      <c r="M9" s="86">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="24" customHeight="1">
+      <c r="A10" s="86">
+        <v>12</v>
+      </c>
+      <c r="B10" s="86" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="86" t="s">
+        <v>757</v>
+      </c>
+      <c r="D10" s="86" t="s">
+        <v>269</v>
+      </c>
+      <c r="E10" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="87" t="s">
+        <v>758</v>
+      </c>
+      <c r="G10" s="86" t="s">
+        <v>759</v>
+      </c>
+      <c r="H10" s="85"/>
+      <c r="I10" s="86" t="s">
+        <v>760</v>
+      </c>
+      <c r="J10" s="86" t="s">
+        <v>756</v>
+      </c>
+      <c r="K10" s="85"/>
+      <c r="L10" s="86">
+        <v>504</v>
+      </c>
+      <c r="M10" s="86">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="4">
@@ -15474,7 +15599,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F9" r:id="rId1" tooltip="https://apicast-pagos-3scale.uatapps.dombif.peru" display="https://apicast-pagos-3scale.uatapps.dombif.peru/" xr:uid="{F1AD885B-2682-431F-AA9B-86A50B2BA8AF}"/>
+    <hyperlink ref="F10" r:id="rId2" tooltip="https://apicast-pagos-3scale.uatapps.dombif.peru:443" display="https://apicast-pagos-3scale.uatapps.dombif.peru/" xr:uid="{FC317455-46FC-46D2-8FA3-E228466A065A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -18196,7 +18326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F92DF8-EE37-4109-A8E4-C6A4AFD03D65}">
   <dimension ref="A1:GA62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="K36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -28300,7 +28430,7 @@
     <row r="8" spans="2:7">
       <c r="B8">
         <f ca="1">RANDBETWEEN(200,400)</f>
-        <v>304</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="177" customHeight="1">
@@ -33692,10 +33822,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76A4116-C805-4C7A-9D35-3A7EDAC4124A}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -33846,6 +33976,29 @@
         <v>425</v>
       </c>
     </row>
+    <row r="7" spans="1:7" ht="33">
+      <c r="A7" s="88">
+        <v>6</v>
+      </c>
+      <c r="B7" s="88" t="s">
+        <v>761</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>762</v>
+      </c>
+      <c r="D7" s="87" t="s">
+        <v>763</v>
+      </c>
+      <c r="E7" s="86" t="s">
+        <v>764</v>
+      </c>
+      <c r="F7" s="88" t="s">
+        <v>765</v>
+      </c>
+      <c r="G7" s="88" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="8" spans="1:7">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -33873,10 +34026,6 @@
     <row r="14" spans="1:7">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -33884,8 +34033,9 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{25EAD435-9A9F-4F5C-858C-3EDC06ED2A93}"/>
     <hyperlink ref="D6" r:id="rId3" xr:uid="{18DBAB1D-6EFA-4A90-9A12-A5AD6FB408BA}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{F54C8595-304C-44BC-B57F-9E8F8B841E56}"/>
+    <hyperlink ref="D7" r:id="rId5" tooltip="https://ssorh.uatapps.dombif.peru/" display="https://ssorh.uatapps.dombif.peru/" xr:uid="{D9B0FB36-47EC-444A-81BE-32FCEF416CFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>